<commit_message>
análise de resultados e novas tabelas no relatorio
</commit_message>
<xml_diff>
--- a/Resultados/Resultados Finais/Algoritmos.xlsx
+++ b/Resultados/Resultados Finais/Algoritmos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\RLP_Qt\Final\Resultados Finais\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\RLP_Qt\Resultados\Resultados Finais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8615B2D3-F6DC-4079-A33D-529E71E25F42}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F64C2A-403E-4CEA-91D8-7D5A51521BC9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17910" windowHeight="12150"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17910" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algoritmos" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Algorithm</t>
-  </si>
   <si>
     <t>Time(ms)</t>
   </si>
@@ -43,16 +40,19 @@
     <t>Custom Algorithm</t>
   </si>
   <si>
-    <t>Genetic Algorithm</t>
+    <t>Ant Colony Optimization</t>
   </si>
   <si>
-    <t>Ant Colony Optimization</t>
+    <t>Algoritmo Genético</t>
+  </si>
+  <si>
+    <t>Algoritmo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,11 +551,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Cor1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -910,40 +911,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="A1:E5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>5752.8784876649397</v>
@@ -960,28 +962,36 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>293.81508892713703</v>
+      </c>
+      <c r="C3" s="3">
+        <v>25.449044320137599</v>
+      </c>
+      <c r="D3" s="2">
+        <v>738.99285714285702</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4.9189285714285704</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
-        <v>293.81508892713703</v>
-      </c>
-      <c r="C4" s="3">
-        <v>25.449044320137599</v>
+      <c r="B4" s="2">
+        <v>6540.4494637690204</v>
+      </c>
+      <c r="C4" s="2">
+        <v>53.399727705482498</v>
       </c>
       <c r="D4" s="2">
-        <v>738.99285714285702</v>
-      </c>
-      <c r="E4" s="2">
-        <v>4.9189285714285704</v>
+        <v>792.92280314099298</v>
+      </c>
+      <c r="E4" s="4">
+        <v>5.0716435671684197</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -994,7 +1004,7 @@
       <c r="C5" s="2">
         <v>61.813138841078597</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>777.28214285714296</v>
       </c>
       <c r="E5" s="2">
@@ -1003,5 +1013,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>